<commit_message>
log + input validation
</commit_message>
<xml_diff>
--- a/doc/Security Control and Threat Analysis/Threat analysis & Control baseline.xlsx
+++ b/doc/Security Control and Threat Analysis/Threat analysis & Control baseline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FileHistory\forza\LAPTOP-NTLPUK8E\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuse\Universita\SecureSystemDesign2022\Progetto\LightingOrder\doc\Security Control and Threat Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9730C03-D21B-4F29-9B1A-7E405AE718BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A329F2C-1D7E-436A-831A-434E92C4C355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threats" sheetId="4" r:id="rId1"/>
@@ -2172,9 +2172,6 @@
   </si>
   <si>
     <t>APPLICATION PARTITIONING</t>
-  </si>
-  <si>
-    <t>Keycloak fornisce una interfaccia separata per l'admin,xosi come Vault e l'applicazione Android. Per quanto riguarda i Proxy ecc sono dei servizi locali. Per la connessione al database è utilizzato il servizio AWS RDS. Quindi è stata realizzata la separazione delle funzionalità. Ogni Proxy ha il proprio indirizzo IP, ogni componente lavora su indirizzi diversi.</t>
   </si>
   <si>
     <t>SC-3</t>
@@ -2868,6 +2865,9 @@
   </si>
   <si>
     <t>SI-8 (1) (2)</t>
+  </si>
+  <si>
+    <t>Keycloak fornisce una interfaccia separata per l'admin, così come Vault e l'applicazione Android. Per quanto riguarda i Proxy ecc sono dei servizi locali. Per la connessione al database è utilizzato il servizio AWS RDS. Quindi è stata realizzata la separazione delle funzionalità. Ogni Proxy ha il proprio indirizzo IP, ogni componente lavora su indirizzi diversi.</t>
   </si>
 </sst>
 </file>
@@ -3575,6 +3575,72 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3586,72 +3652,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4253,28 +4253,28 @@
       <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="25"/>
-    <col min="2" max="2" width="22.85546875" style="25" customWidth="1"/>
-    <col min="3" max="4" width="47.85546875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="105.5703125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="56.5703125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="51.42578125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="25"/>
+    <col min="2" max="2" width="22.88671875" style="25" customWidth="1"/>
+    <col min="3" max="4" width="47.88671875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="105.5546875" style="25" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="56.5546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="51.44140625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="84"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="106"/>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
@@ -4295,7 +4295,7 @@
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -4340,7 +4340,7 @@
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
     </row>
-    <row r="3" spans="1:27" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="80" t="s">
         <v>9</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>17</v>
       </c>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>25</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="66" t="s">
         <v>31</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="66" t="s">
         <v>37</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="66" t="s">
         <v>43</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="66" t="s">
         <v>44</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66" t="s">
         <v>49</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>52</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
         <v>56</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
         <v>59</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="66" t="s">
         <v>60</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="66" t="s">
         <v>67</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
         <v>72</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="66" t="s">
         <v>78</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="66" t="s">
         <v>83</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="66" t="s">
         <v>88</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="66" t="s">
         <v>95</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="66" t="s">
         <v>98</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="66" t="s">
         <v>104</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
         <v>109</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="71" t="s">
         <v>114</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="71" t="s">
         <v>119</v>
       </c>
@@ -4928,7 +4928,7 @@
       </c>
       <c r="J25" s="24"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="71" t="s">
         <v>123</v>
       </c>
@@ -4953,7 +4953,7 @@
       </c>
       <c r="J26" s="24"/>
     </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="71" t="s">
         <v>126</v>
       </c>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="J27" s="24"/>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="71" t="s">
         <v>127</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="71" t="s">
         <v>133</v>
       </c>
@@ -5029,7 +5029,7 @@
       </c>
       <c r="J29" s="24"/>
     </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="71" t="s">
         <v>134</v>
       </c>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="J30" s="24"/>
     </row>
-    <row r="31" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
         <v>139</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="73" t="s">
         <v>142</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="73" t="s">
         <v>147</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="77" t="s">
         <v>152</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="77" t="s">
         <v>158</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="77" t="s">
         <v>163</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="77" t="s">
         <v>167</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="81" t="s">
         <v>170</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="81" t="s">
         <v>173</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="81" t="s">
         <v>177</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="79" t="s">
         <v>181</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="79" t="s">
         <v>185</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="79" t="s">
         <v>187</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="79" t="s">
         <v>189</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="79" t="s">
         <v>192</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="79" t="s">
         <v>194</v>
       </c>
@@ -5493,20 +5493,20 @@
       <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" customWidth="1"/>
     <col min="3" max="3" width="74" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -5529,7 +5529,7 @@
       <c r="Y1" s="15"/>
       <c r="Z1" s="15"/>
     </row>
-    <row r="2" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -5565,7 +5565,7 @@
       <c r="Y2" s="17"/>
       <c r="Z2" s="17"/>
     </row>
-    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>198</v>
       </c>
@@ -5601,7 +5601,7 @@
       <c r="Y3" s="18"/>
       <c r="Z3" s="18"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>96</v>
       </c>
@@ -5637,7 +5637,7 @@
       <c r="Y4" s="18"/>
       <c r="Z4" s="18"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>20</v>
       </c>
@@ -5673,7 +5673,7 @@
       <c r="Y5" s="18"/>
       <c r="Z5" s="18"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>50</v>
       </c>
@@ -5709,7 +5709,7 @@
       <c r="Y6" s="18"/>
       <c r="Z6" s="18"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>144</v>
       </c>
@@ -5745,7 +5745,7 @@
       <c r="Y7" s="18"/>
       <c r="Z7" s="18"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>164</v>
       </c>
@@ -5781,7 +5781,7 @@
       <c r="Y8" s="18"/>
       <c r="Z8" s="18"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>90</v>
       </c>
@@ -5817,7 +5817,7 @@
       <c r="Y9" s="18"/>
       <c r="Z9" s="18"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>62</v>
       </c>
@@ -5853,7 +5853,7 @@
       <c r="Y10" s="18"/>
       <c r="Z10" s="18"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>218</v>
       </c>
@@ -5889,7 +5889,7 @@
       <c r="Y11" s="18"/>
       <c r="Z11" s="18"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>121</v>
       </c>
@@ -5925,7 +5925,7 @@
       <c r="Y12" s="18"/>
       <c r="Z12" s="18"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -5953,7 +5953,7 @@
       <c r="Y13" s="18"/>
       <c r="Z13" s="18"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -5981,7 +5981,7 @@
       <c r="Y14" s="18"/>
       <c r="Z14" s="18"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -6009,7 +6009,7 @@
       <c r="Y15" s="18"/>
       <c r="Z15" s="18"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -6037,7 +6037,7 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -6065,7 +6065,7 @@
       <c r="Y17" s="18"/>
       <c r="Z17" s="18"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -6093,7 +6093,7 @@
       <c r="Y18" s="18"/>
       <c r="Z18" s="18"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -6121,7 +6121,7 @@
       <c r="Y19" s="18"/>
       <c r="Z19" s="18"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -6149,7 +6149,7 @@
       <c r="Y20" s="18"/>
       <c r="Z20" s="18"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -6177,7 +6177,7 @@
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -6205,7 +6205,7 @@
       <c r="Y22" s="18"/>
       <c r="Z22" s="18"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -6247,20 +6247,20 @@
   <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.109375" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="82.42578125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="82.44140625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>224</v>
       </c>
@@ -6283,8 +6283,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+    <row r="2" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="82" t="s">
         <v>231</v>
       </c>
       <c r="B2" s="36" t="s">
@@ -6306,8 +6306,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+    <row r="3" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="82" t="s">
         <v>235</v>
       </c>
       <c r="B3" s="39" t="s">
@@ -6319,18 +6319,18 @@
       <c r="D3" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="83" t="s">
+        <v>702</v>
+      </c>
+      <c r="F3" s="84" t="s">
         <v>703</v>
-      </c>
-      <c r="F3" s="88" t="s">
-        <v>704</v>
       </c>
       <c r="G3" s="50" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:7" ht="151.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A4" s="82" t="s">
         <v>238</v>
       </c>
       <c r="B4" s="36" t="s">
@@ -6352,8 +6352,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="86" t="s">
+    <row r="5" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="82" t="s">
         <v>241</v>
       </c>
       <c r="B5" s="39" t="s">
@@ -6373,8 +6373,8 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="86" t="s">
+    <row r="6" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="82" t="s">
         <v>244</v>
       </c>
       <c r="B6" s="36" t="s">
@@ -6384,18 +6384,18 @@
         <v>233</v>
       </c>
       <c r="D6" s="36"/>
-      <c r="E6" s="89" t="s">
+      <c r="E6" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="F6" s="90" t="s">
+      <c r="F6" s="86" t="s">
         <v>244</v>
       </c>
       <c r="G6" s="48" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A7" s="86" t="s">
+    <row r="7" spans="1:7" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="82" t="s">
         <v>247</v>
       </c>
       <c r="B7" s="39" t="s">
@@ -6405,18 +6405,18 @@
         <v>233</v>
       </c>
       <c r="D7" s="39"/>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="87" t="s">
+        <v>704</v>
+      </c>
+      <c r="F7" s="51" t="s">
         <v>705</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>706</v>
       </c>
       <c r="G7" s="50" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="86" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="82" t="s">
         <v>250</v>
       </c>
       <c r="B8" s="36" t="s">
@@ -6438,8 +6438,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="86" t="s">
+    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="82" t="s">
         <v>254</v>
       </c>
       <c r="B9" s="39" t="s">
@@ -6461,8 +6461,8 @@
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="82" t="s">
         <v>257</v>
       </c>
       <c r="B10" s="36" t="s">
@@ -6480,8 +6480,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="86" t="s">
+    <row r="11" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="82" t="s">
         <v>261</v>
       </c>
       <c r="B11" s="39" t="s">
@@ -6501,8 +6501,8 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="86" t="s">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="82" t="s">
         <v>265</v>
       </c>
       <c r="B12" s="36" t="s">
@@ -6522,8 +6522,8 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="86" t="s">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="82" t="s">
         <v>268</v>
       </c>
       <c r="B13" s="39" t="s">
@@ -6532,21 +6532,21 @@
       <c r="C13" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="88" t="s">
         <v>268</v>
       </c>
       <c r="E13" s="41" t="s">
         <v>268</v>
       </c>
-      <c r="F13" s="93" t="s">
+      <c r="F13" s="89" t="s">
         <v>268</v>
       </c>
       <c r="G13" s="50" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="86" t="s">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="82" t="s">
         <v>271</v>
       </c>
       <c r="B14" s="36" t="s">
@@ -6558,18 +6558,18 @@
       <c r="D14" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="E14" s="94" t="s">
+      <c r="E14" s="90" t="s">
+        <v>706</v>
+      </c>
+      <c r="F14" s="91" t="s">
         <v>707</v>
-      </c>
-      <c r="F14" s="95" t="s">
-        <v>708</v>
       </c>
       <c r="G14" s="48" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="86" t="s">
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="82" t="s">
         <v>274</v>
       </c>
       <c r="B15" s="39" t="s">
@@ -6581,18 +6581,18 @@
       <c r="D15" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E15" s="92" t="s">
         <v>276</v>
       </c>
-      <c r="F15" s="93" t="s">
-        <v>709</v>
+      <c r="F15" s="89" t="s">
+        <v>708</v>
       </c>
       <c r="G15" s="50" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="86" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="82" t="s">
         <v>278</v>
       </c>
       <c r="B16" s="36" t="s">
@@ -6604,18 +6604,18 @@
       <c r="D16" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="E16" s="97" t="s">
+      <c r="E16" s="93" t="s">
         <v>280</v>
       </c>
-      <c r="F16" s="97" t="s">
+      <c r="F16" s="93" t="s">
         <v>280</v>
       </c>
       <c r="G16" s="54" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="86" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="82" t="s">
         <v>281</v>
       </c>
       <c r="B17" s="39" t="s">
@@ -6627,18 +6627,18 @@
       <c r="D17" s="39" t="s">
         <v>281</v>
       </c>
-      <c r="E17" s="92" t="s">
-        <v>711</v>
-      </c>
-      <c r="F17" s="93" t="s">
-        <v>711</v>
+      <c r="E17" s="88" t="s">
+        <v>710</v>
+      </c>
+      <c r="F17" s="89" t="s">
+        <v>710</v>
       </c>
       <c r="G17" s="54" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="86" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="82" t="s">
         <v>284</v>
       </c>
       <c r="B18" s="36" t="s">
@@ -6648,7 +6648,7 @@
         <v>252</v>
       </c>
       <c r="D18" s="36"/>
-      <c r="E18" s="89" t="s">
+      <c r="E18" s="85" t="s">
         <v>284</v>
       </c>
       <c r="F18" s="52" t="s">
@@ -6658,8 +6658,8 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="86" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="82" t="s">
         <v>286</v>
       </c>
       <c r="B19" s="39" t="s">
@@ -6668,7 +6668,7 @@
       <c r="C19" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="D19" s="91" t="s">
+      <c r="D19" s="87" t="s">
         <v>286</v>
       </c>
       <c r="E19" s="39" t="s">
@@ -6681,8 +6681,8 @@
         <v>583</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="86" t="s">
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="82" t="s">
         <v>288</v>
       </c>
       <c r="B20" s="36" t="s">
@@ -6702,8 +6702,8 @@
       </c>
       <c r="G20" s="53"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="86" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="82" t="s">
         <v>290</v>
       </c>
       <c r="B21" s="39" t="s">
@@ -6723,8 +6723,8 @@
       </c>
       <c r="G21" s="53"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="86" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="82" t="s">
         <v>293</v>
       </c>
       <c r="B22" s="36" t="s">
@@ -6744,8 +6744,8 @@
       </c>
       <c r="G22" s="53"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="86" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="82" t="s">
         <v>295</v>
       </c>
       <c r="B23" s="39" t="s">
@@ -6765,8 +6765,8 @@
       </c>
       <c r="G23" s="53"/>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="86" t="s">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="82" t="s">
         <v>297</v>
       </c>
       <c r="B24" s="36" t="s">
@@ -6788,8 +6788,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="86" t="s">
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="82" t="s">
         <v>299</v>
       </c>
       <c r="B25" s="39" t="s">
@@ -6801,18 +6801,18 @@
       <c r="D25" s="41" t="s">
         <v>299</v>
       </c>
-      <c r="E25" s="97" t="s">
+      <c r="E25" s="93" t="s">
         <v>301</v>
       </c>
-      <c r="F25" s="97" t="s">
+      <c r="F25" s="93" t="s">
         <v>301</v>
       </c>
       <c r="G25" s="54" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="86" t="s">
+    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="82" t="s">
         <v>303</v>
       </c>
       <c r="B26" s="36" t="s">
@@ -6824,18 +6824,18 @@
       <c r="D26" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="E26" s="98" t="s">
+      <c r="E26" s="94" t="s">
         <v>305</v>
       </c>
       <c r="F26" s="65" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G26" s="48" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="86" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="82" t="s">
         <v>307</v>
       </c>
       <c r="B27" s="39" t="s">
@@ -6844,7 +6844,7 @@
       <c r="C27" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="D27" s="92" t="s">
+      <c r="D27" s="88" t="s">
         <v>307</v>
       </c>
       <c r="E27" s="41" t="s">
@@ -6857,8 +6857,8 @@
         <v>309</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="86" t="s">
+    <row r="28" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="82" t="s">
         <v>310</v>
       </c>
       <c r="B28" s="36" t="s">
@@ -6867,21 +6867,21 @@
       <c r="C28" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="D28" s="89" t="s">
+      <c r="D28" s="85" t="s">
         <v>310</v>
       </c>
       <c r="E28" s="36" t="s">
         <v>310</v>
       </c>
       <c r="F28" s="65" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G28" s="48" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="86" t="s">
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="82" t="s">
         <v>313</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -6893,18 +6893,18 @@
       <c r="D29" s="41" t="s">
         <v>313</v>
       </c>
-      <c r="E29" s="92" t="s">
+      <c r="E29" s="88" t="s">
+        <v>713</v>
+      </c>
+      <c r="F29" s="89" t="s">
         <v>714</v>
-      </c>
-      <c r="F29" s="93" t="s">
-        <v>715</v>
       </c>
       <c r="G29" s="48" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="86" t="s">
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="82" t="s">
         <v>316</v>
       </c>
       <c r="B30" s="36" t="s">
@@ -6914,18 +6914,18 @@
         <v>252</v>
       </c>
       <c r="D30" s="36"/>
-      <c r="E30" s="99" t="s">
+      <c r="E30" s="95" t="s">
         <v>318</v>
       </c>
-      <c r="F30" s="97" t="s">
+      <c r="F30" s="93" t="s">
         <v>318</v>
       </c>
       <c r="G30" s="48" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="86" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="82" t="s">
         <v>320</v>
       </c>
       <c r="B31" s="39" t="s">
@@ -6947,8 +6947,8 @@
         <v>323</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="86" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="82" t="s">
         <v>324</v>
       </c>
       <c r="B32" s="36" t="s">
@@ -6960,18 +6960,18 @@
       <c r="D32" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="E32" s="100" t="s">
+      <c r="E32" s="96" t="s">
         <v>326</v>
       </c>
       <c r="F32" s="65" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G32" s="48" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="86" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="82" t="s">
         <v>328</v>
       </c>
       <c r="B33" s="39" t="s">
@@ -6989,8 +6989,8 @@
         <v>330</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="86" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="82" t="s">
         <v>331</v>
       </c>
       <c r="B34" s="36" t="s">
@@ -7012,8 +7012,8 @@
         <v>333</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="86" t="s">
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="82" t="s">
         <v>334</v>
       </c>
       <c r="B35" s="39" t="s">
@@ -7028,15 +7028,15 @@
       <c r="E35" s="41" t="s">
         <v>334</v>
       </c>
-      <c r="F35" s="93" t="s">
+      <c r="F35" s="89" t="s">
+        <v>716</v>
+      </c>
+      <c r="G35" s="48" t="s">
         <v>717</v>
       </c>
-      <c r="G35" s="48" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="86" t="s">
+    </row>
+    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="82" t="s">
         <v>336</v>
       </c>
       <c r="B36" s="36" t="s">
@@ -7056,8 +7056,8 @@
       </c>
       <c r="G36"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="86" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="82" t="s">
         <v>338</v>
       </c>
       <c r="B37" s="39" t="s">
@@ -7077,8 +7077,8 @@
       </c>
       <c r="G37"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="86" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="82" t="s">
         <v>342</v>
       </c>
       <c r="B38" s="36" t="s">
@@ -7098,8 +7098,8 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="86" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="82" t="s">
         <v>345</v>
       </c>
       <c r="B39" s="39" t="s">
@@ -7119,8 +7119,8 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="86" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="82" t="s">
         <v>347</v>
       </c>
       <c r="B40" s="36" t="s">
@@ -7140,8 +7140,8 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="86" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="82" t="s">
         <v>349</v>
       </c>
       <c r="B41" s="39" t="s">
@@ -7161,8 +7161,8 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="86" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="82" t="s">
         <v>352</v>
       </c>
       <c r="B42" s="36" t="s">
@@ -7178,8 +7178,8 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="86" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="82" t="s">
         <v>354</v>
       </c>
       <c r="B43" s="39" t="s">
@@ -7199,8 +7199,8 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="86" t="s">
+    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="82" t="s">
         <v>356</v>
       </c>
       <c r="B44" s="36" t="s">
@@ -7220,8 +7220,8 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="86" t="s">
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="82" t="s">
         <v>358</v>
       </c>
       <c r="B45" s="39" t="s">
@@ -7233,16 +7233,16 @@
       <c r="D45" s="39" t="s">
         <v>358</v>
       </c>
-      <c r="E45" s="92" t="s">
+      <c r="E45" s="88" t="s">
+        <v>718</v>
+      </c>
+      <c r="F45" s="88" t="s">
         <v>719</v>
       </c>
-      <c r="F45" s="92" t="s">
-        <v>720</v>
-      </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="86" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="82" t="s">
         <v>360</v>
       </c>
       <c r="B46" s="36" t="s">
@@ -7252,16 +7252,16 @@
         <v>233</v>
       </c>
       <c r="D46" s="36"/>
-      <c r="E46" s="97" t="s">
+      <c r="E46" s="93" t="s">
         <v>362</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="86" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="82" t="s">
         <v>363</v>
       </c>
       <c r="B47" s="39" t="s">
@@ -7281,8 +7281,8 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="86" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="82" t="s">
         <v>366</v>
       </c>
       <c r="B48" s="36" t="s">
@@ -7296,12 +7296,12 @@
         <v>366</v>
       </c>
       <c r="F48" s="42" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="86" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="82" t="s">
         <v>368</v>
       </c>
       <c r="B49" s="39" t="s">
@@ -7316,13 +7316,13 @@
       <c r="E49" s="39" t="s">
         <v>368</v>
       </c>
-      <c r="F49" s="92" t="s">
-        <v>723</v>
+      <c r="F49" s="88" t="s">
+        <v>722</v>
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="86" t="s">
+    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="82" t="s">
         <v>370</v>
       </c>
       <c r="B50" s="36" t="s">
@@ -7335,15 +7335,15 @@
         <v>370</v>
       </c>
       <c r="E50" s="42" t="s">
+        <v>723</v>
+      </c>
+      <c r="F50" s="42" t="s">
         <v>724</v>
       </c>
-      <c r="F50" s="42" t="s">
-        <v>725</v>
-      </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="86" t="s">
+    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="82" t="s">
         <v>372</v>
       </c>
       <c r="B51" s="39" t="s">
@@ -7355,16 +7355,16 @@
       <c r="D51" s="39" t="s">
         <v>372</v>
       </c>
-      <c r="E51" s="92" t="s">
+      <c r="E51" s="88" t="s">
+        <v>725</v>
+      </c>
+      <c r="F51" s="88" t="s">
         <v>726</v>
       </c>
-      <c r="F51" s="92" t="s">
-        <v>727</v>
-      </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="86" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="82" t="s">
         <v>374</v>
       </c>
       <c r="B52" s="36" t="s">
@@ -7382,8 +7382,8 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="86" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="82" t="s">
         <v>376</v>
       </c>
       <c r="B53" s="39" t="s">
@@ -7403,8 +7403,8 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="86" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="82" t="s">
         <v>378</v>
       </c>
       <c r="B54" s="36" t="s">
@@ -7424,8 +7424,8 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="86" t="s">
+    <row r="55" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="82" t="s">
         <v>380</v>
       </c>
       <c r="B55" s="39" t="s">
@@ -7447,8 +7447,8 @@
         <v>382</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A56" s="86" t="s">
+    <row r="56" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="82" t="s">
         <v>383</v>
       </c>
       <c r="B56" s="36" t="s">
@@ -7460,18 +7460,18 @@
       <c r="D56" s="38" t="s">
         <v>383</v>
       </c>
-      <c r="E56" s="89" t="s">
+      <c r="E56" s="85" t="s">
+        <v>727</v>
+      </c>
+      <c r="F56" s="65" t="s">
         <v>728</v>
-      </c>
-      <c r="F56" s="65" t="s">
-        <v>729</v>
       </c>
       <c r="G56" s="48" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="86" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="82" t="s">
         <v>386</v>
       </c>
       <c r="B57" s="39" t="s">
@@ -7486,15 +7486,15 @@
       <c r="E57" s="39" t="s">
         <v>386</v>
       </c>
-      <c r="F57" s="97" t="s">
+      <c r="F57" s="93" t="s">
         <v>388</v>
       </c>
       <c r="G57" s="50" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="86" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="82" t="s">
         <v>390</v>
       </c>
       <c r="B58" s="36" t="s">
@@ -7506,18 +7506,18 @@
       <c r="D58" s="38" t="s">
         <v>390</v>
       </c>
-      <c r="E58" s="97" t="s">
+      <c r="E58" s="93" t="s">
         <v>392</v>
       </c>
-      <c r="F58" s="101" t="s">
-        <v>730</v>
+      <c r="F58" s="97" t="s">
+        <v>729</v>
       </c>
       <c r="G58" s="48" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A59" s="86" t="s">
+    <row r="59" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="82" t="s">
         <v>394</v>
       </c>
       <c r="B59" s="39" t="s">
@@ -7537,8 +7537,8 @@
         <v>398</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="86" t="s">
+    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="82" t="s">
         <v>399</v>
       </c>
       <c r="B60" s="36" t="s">
@@ -7548,18 +7548,18 @@
         <v>233</v>
       </c>
       <c r="D60" s="36"/>
-      <c r="E60" s="94" t="s">
+      <c r="E60" s="90" t="s">
+        <v>730</v>
+      </c>
+      <c r="F60" s="97" t="s">
         <v>731</v>
-      </c>
-      <c r="F60" s="101" t="s">
-        <v>732</v>
       </c>
       <c r="G60" s="48" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="86" t="s">
+    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="82" t="s">
         <v>402</v>
       </c>
       <c r="B61" s="39" t="s">
@@ -7569,18 +7569,18 @@
         <v>233</v>
       </c>
       <c r="D61" s="39"/>
-      <c r="E61" s="87" t="s">
+      <c r="E61" s="83" t="s">
+        <v>732</v>
+      </c>
+      <c r="F61" s="84" t="s">
         <v>733</v>
-      </c>
-      <c r="F61" s="88" t="s">
-        <v>734</v>
       </c>
       <c r="G61" s="48" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A62" s="86" t="s">
+    <row r="62" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A62" s="82" t="s">
         <v>405</v>
       </c>
       <c r="B62" s="36" t="s">
@@ -7592,7 +7592,7 @@
       <c r="D62" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="E62" s="97" t="s">
+      <c r="E62" s="93" t="s">
         <v>407</v>
       </c>
       <c r="F62" s="49" t="s">
@@ -7602,8 +7602,8 @@
         <v>409</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="86" t="s">
+    <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="82" t="s">
         <v>410</v>
       </c>
       <c r="B63" s="39" t="s">
@@ -7618,15 +7618,15 @@
       <c r="E63" s="43" t="s">
         <v>412</v>
       </c>
-      <c r="F63" s="88" t="s">
-        <v>735</v>
+      <c r="F63" s="84" t="s">
+        <v>734</v>
       </c>
       <c r="G63" s="48" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A64" s="86" t="s">
+    <row r="64" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="82" t="s">
         <v>414</v>
       </c>
       <c r="B64" s="30" t="s">
@@ -7648,8 +7648,8 @@
         <v>416</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A65" s="86" t="s">
+    <row r="65" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="82" t="s">
         <v>417</v>
       </c>
       <c r="B65" s="27" t="s">
@@ -7659,20 +7659,20 @@
         <v>233</v>
       </c>
       <c r="D65" s="29" t="s">
+        <v>735</v>
+      </c>
+      <c r="E65" s="29" t="s">
         <v>736</v>
       </c>
-      <c r="E65" s="29" t="s">
+      <c r="F65" s="98" t="s">
         <v>737</v>
-      </c>
-      <c r="F65" s="102" t="s">
-        <v>738</v>
       </c>
       <c r="G65" s="60" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A66" s="86" t="s">
+    <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="82" t="s">
         <v>420</v>
       </c>
       <c r="B66" s="30" t="s">
@@ -7694,8 +7694,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="86" t="s">
+    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="82" t="s">
         <v>424</v>
       </c>
       <c r="B67" s="27" t="s">
@@ -7717,8 +7717,8 @@
         <v>426</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A68" s="86" t="s">
+    <row r="68" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="82" t="s">
         <v>427</v>
       </c>
       <c r="B68" s="30" t="s">
@@ -7727,21 +7727,21 @@
       <c r="C68" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="D68" s="103" t="s">
+      <c r="D68" s="99" t="s">
+        <v>738</v>
+      </c>
+      <c r="E68" s="99" t="s">
         <v>739</v>
       </c>
-      <c r="E68" s="103" t="s">
+      <c r="F68" s="100" t="s">
         <v>740</v>
-      </c>
-      <c r="F68" s="104" t="s">
-        <v>741</v>
       </c>
       <c r="G68" s="59" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="86" t="s">
+    <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="82" t="s">
         <v>430</v>
       </c>
       <c r="B69" s="27" t="s">
@@ -7756,15 +7756,15 @@
       <c r="E69" s="29" t="s">
         <v>430</v>
       </c>
-      <c r="F69" s="105" t="s">
+      <c r="F69" s="101" t="s">
         <v>430</v>
       </c>
       <c r="G69" s="60" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="86" t="s">
+    <row r="70" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="82" t="s">
         <v>433</v>
       </c>
       <c r="B70" s="30" t="s">
@@ -7786,8 +7786,8 @@
         <v>435</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="86" t="s">
+    <row r="71" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="82" t="s">
         <v>436</v>
       </c>
       <c r="B71" s="27" t="s">
@@ -7796,21 +7796,21 @@
       <c r="C71" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="D71" s="106" t="s">
-        <v>742</v>
-      </c>
-      <c r="E71" s="106" t="s">
-        <v>742</v>
-      </c>
-      <c r="F71" s="105" t="s">
-        <v>742</v>
+      <c r="D71" s="102" t="s">
+        <v>741</v>
+      </c>
+      <c r="E71" s="102" t="s">
+        <v>741</v>
+      </c>
+      <c r="F71" s="101" t="s">
+        <v>741</v>
       </c>
       <c r="G71" s="60" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="107" t="s">
+    <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A72" s="103" t="s">
         <v>439</v>
       </c>
       <c r="B72" s="27" t="s">
@@ -7832,8 +7832,8 @@
         <v>422</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="107" t="s">
+    <row r="73" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="103" t="s">
         <v>442</v>
       </c>
       <c r="B73" s="27" t="s">
@@ -7855,8 +7855,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="107" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="103" t="s">
         <v>445</v>
       </c>
       <c r="B74" s="27" t="s">
@@ -7878,8 +7878,8 @@
         <v>422</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="86" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="82" t="s">
         <v>447</v>
       </c>
       <c r="B75" s="39" t="s">
@@ -7899,8 +7899,8 @@
       </c>
       <c r="G75"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="86" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="82" t="s">
         <v>451</v>
       </c>
       <c r="B76" s="36" t="s">
@@ -7920,8 +7920,8 @@
       </c>
       <c r="G76"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="86" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="82" t="s">
         <v>454</v>
       </c>
       <c r="B77" s="39" t="s">
@@ -7941,8 +7941,8 @@
       </c>
       <c r="G77"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="86" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="82" t="s">
         <v>457</v>
       </c>
       <c r="B78" s="36" t="s">
@@ -7962,8 +7962,8 @@
       </c>
       <c r="G78"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="86" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="82" t="s">
         <v>460</v>
       </c>
       <c r="B79" s="39" t="s">
@@ -7983,8 +7983,8 @@
       </c>
       <c r="G79"/>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="86" t="s">
+    <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="82" t="s">
         <v>462</v>
       </c>
       <c r="B80" s="36" t="s">
@@ -8004,8 +8004,8 @@
       </c>
       <c r="G80"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="86" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="82" t="s">
         <v>464</v>
       </c>
       <c r="B81" s="39" t="s">
@@ -8025,8 +8025,8 @@
       </c>
       <c r="G81"/>
     </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="86" t="s">
+    <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="82" t="s">
         <v>467</v>
       </c>
       <c r="B82" s="36" t="s">
@@ -8037,15 +8037,15 @@
       </c>
       <c r="D82" s="36"/>
       <c r="E82" s="42" t="s">
+        <v>742</v>
+      </c>
+      <c r="F82" s="42" t="s">
         <v>743</v>
       </c>
-      <c r="F82" s="42" t="s">
-        <v>744</v>
-      </c>
       <c r="G82"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="86" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="82" t="s">
         <v>469</v>
       </c>
       <c r="B83" s="39" t="s">
@@ -8065,8 +8065,8 @@
       </c>
       <c r="G83"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="86" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="82" t="s">
         <v>473</v>
       </c>
       <c r="B84" s="36" t="s">
@@ -8086,8 +8086,8 @@
       </c>
       <c r="G84"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="86" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="82" t="s">
         <v>476</v>
       </c>
       <c r="B85" s="39" t="s">
@@ -8105,8 +8105,8 @@
       </c>
       <c r="G85"/>
     </row>
-    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="86" t="s">
+    <row r="86" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="82" t="s">
         <v>478</v>
       </c>
       <c r="B86" s="36" t="s">
@@ -8126,8 +8126,8 @@
       </c>
       <c r="G86"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="86" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="82" t="s">
         <v>480</v>
       </c>
       <c r="B87" s="39" t="s">
@@ -8147,8 +8147,8 @@
       </c>
       <c r="G87"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="86" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="82" t="s">
         <v>482</v>
       </c>
       <c r="B88" s="36" t="s">
@@ -8166,8 +8166,8 @@
       </c>
       <c r="G88"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="86" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="82" t="s">
         <v>484</v>
       </c>
       <c r="B89" s="39" t="s">
@@ -8185,8 +8185,8 @@
       </c>
       <c r="G89"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="86" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="82" t="s">
         <v>486</v>
       </c>
       <c r="B90" s="36" t="s">
@@ -8204,8 +8204,8 @@
       </c>
       <c r="G90"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="86" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="82" t="s">
         <v>489</v>
       </c>
       <c r="B91" s="39" t="s">
@@ -8225,8 +8225,8 @@
       </c>
       <c r="G91"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="86" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="82" t="s">
         <v>492</v>
       </c>
       <c r="B92" s="36" t="s">
@@ -8246,8 +8246,8 @@
       </c>
       <c r="G92"/>
     </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="86" t="s">
+    <row r="93" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A93" s="82" t="s">
         <v>495</v>
       </c>
       <c r="B93" s="39" t="s">
@@ -8267,8 +8267,8 @@
       </c>
       <c r="G93"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="86" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="82" t="s">
         <v>497</v>
       </c>
       <c r="B94" s="36" t="s">
@@ -8288,8 +8288,8 @@
       </c>
       <c r="G94"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="86" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="82" t="s">
         <v>499</v>
       </c>
       <c r="B95" s="39" t="s">
@@ -8309,8 +8309,8 @@
       </c>
       <c r="G95"/>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="86" t="s">
+    <row r="96" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="82" t="s">
         <v>502</v>
       </c>
       <c r="B96" s="36" t="s">
@@ -8328,8 +8328,8 @@
       </c>
       <c r="G96"/>
     </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="86" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" s="82" t="s">
         <v>504</v>
       </c>
       <c r="B97" s="39" t="s">
@@ -8347,8 +8347,8 @@
       </c>
       <c r="G97"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="86" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98" s="82" t="s">
         <v>506</v>
       </c>
       <c r="B98" s="36" t="s">
@@ -8368,8 +8368,8 @@
       </c>
       <c r="G98"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="86" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="82" t="s">
         <v>510</v>
       </c>
       <c r="B99" s="39" t="s">
@@ -8389,8 +8389,8 @@
       </c>
       <c r="G99"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="86" t="s">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="82" t="s">
         <v>513</v>
       </c>
       <c r="B100" s="36" t="s">
@@ -8408,8 +8408,8 @@
       </c>
       <c r="G100"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="86" t="s">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="82" t="s">
         <v>515</v>
       </c>
       <c r="B101" s="39" t="s">
@@ -8427,8 +8427,8 @@
       </c>
       <c r="G101"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="86" t="s">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="82" t="s">
         <v>517</v>
       </c>
       <c r="B102" s="36" t="s">
@@ -8446,8 +8446,8 @@
       </c>
       <c r="G102"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="86" t="s">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="82" t="s">
         <v>520</v>
       </c>
       <c r="B103" s="39" t="s">
@@ -8467,8 +8467,8 @@
       </c>
       <c r="G103"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="86" t="s">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="82" t="s">
         <v>522</v>
       </c>
       <c r="B104" s="36" t="s">
@@ -8484,12 +8484,12 @@
         <v>524</v>
       </c>
       <c r="F104" s="42" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G104"/>
     </row>
-    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="86" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="82" t="s">
         <v>525</v>
       </c>
       <c r="B105" s="39" t="s">
@@ -8509,8 +8509,8 @@
       </c>
       <c r="G105"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="86" t="s">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="82" t="s">
         <v>527</v>
       </c>
       <c r="B106" s="36" t="s">
@@ -8530,8 +8530,8 @@
       </c>
       <c r="G106"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="86" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="82" t="s">
         <v>530</v>
       </c>
       <c r="B107" s="39" t="s">
@@ -8551,8 +8551,8 @@
       </c>
       <c r="G107"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="86" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="82" t="s">
         <v>532</v>
       </c>
       <c r="B108" s="36" t="s">
@@ -8570,8 +8570,8 @@
       </c>
       <c r="G108"/>
     </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="86" t="s">
+    <row r="109" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A109" s="82" t="s">
         <v>534</v>
       </c>
       <c r="B109" s="39" t="s">
@@ -8587,8 +8587,8 @@
       </c>
       <c r="G109"/>
     </row>
-    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="86" t="s">
+    <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A110" s="82" t="s">
         <v>536</v>
       </c>
       <c r="B110" s="36" t="s">
@@ -8608,8 +8608,8 @@
       </c>
       <c r="G110"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="86" t="s">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="82" t="s">
         <v>538</v>
       </c>
       <c r="B111" s="39" t="s">
@@ -8629,8 +8629,8 @@
       </c>
       <c r="G111"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="86" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="82" t="s">
         <v>541</v>
       </c>
       <c r="B112" s="36" t="s">
@@ -8650,8 +8650,8 @@
       </c>
       <c r="G112"/>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="86" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="82" t="s">
         <v>544</v>
       </c>
       <c r="B113" s="39" t="s">
@@ -8669,8 +8669,8 @@
       </c>
       <c r="G113"/>
     </row>
-    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="86" t="s">
+    <row r="114" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="82" t="s">
         <v>546</v>
       </c>
       <c r="B114" s="36" t="s">
@@ -8690,8 +8690,8 @@
       </c>
       <c r="G114"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="86" t="s">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="82" t="s">
         <v>548</v>
       </c>
       <c r="B115" s="39" t="s">
@@ -8711,8 +8711,8 @@
       </c>
       <c r="G115"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="86" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" s="82" t="s">
         <v>550</v>
       </c>
       <c r="B116" s="36" t="s">
@@ -8732,8 +8732,8 @@
       </c>
       <c r="G116"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="86" t="s">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" s="82" t="s">
         <v>552</v>
       </c>
       <c r="B117" s="39" t="s">
@@ -8753,8 +8753,8 @@
       </c>
       <c r="G117"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="86" t="s">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="82" t="s">
         <v>555</v>
       </c>
       <c r="B118" s="36" t="s">
@@ -8774,8 +8774,8 @@
       </c>
       <c r="G118"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="86" t="s">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="82" t="s">
         <v>557</v>
       </c>
       <c r="B119" s="39" t="s">
@@ -8795,8 +8795,8 @@
       </c>
       <c r="G119"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="86" t="s">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" s="82" t="s">
         <v>559</v>
       </c>
       <c r="B120" s="36" t="s">
@@ -8816,8 +8816,8 @@
       </c>
       <c r="G120"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="86" t="s">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" s="82" t="s">
         <v>561</v>
       </c>
       <c r="B121" s="39" t="s">
@@ -8837,8 +8837,8 @@
       </c>
       <c r="G121"/>
     </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="86" t="s">
+    <row r="122" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A122" s="82" t="s">
         <v>563</v>
       </c>
       <c r="B122" s="36" t="s">
@@ -8858,8 +8858,8 @@
       </c>
       <c r="G122"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="86" t="s">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123" s="82" t="s">
         <v>565</v>
       </c>
       <c r="B123" s="39" t="s">
@@ -8879,8 +8879,8 @@
       </c>
       <c r="G123"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="86" t="s">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124" s="82" t="s">
         <v>567</v>
       </c>
       <c r="B124" s="36" t="s">
@@ -8900,8 +8900,8 @@
       </c>
       <c r="G124"/>
     </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="86" t="s">
+    <row r="125" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="82" t="s">
         <v>569</v>
       </c>
       <c r="B125" s="39" t="s">
@@ -8913,16 +8913,16 @@
       <c r="D125" s="39" t="s">
         <v>569</v>
       </c>
-      <c r="E125" s="92" t="s">
+      <c r="E125" s="88" t="s">
+        <v>745</v>
+      </c>
+      <c r="F125" s="88" t="s">
         <v>746</v>
       </c>
-      <c r="F125" s="92" t="s">
-        <v>747</v>
-      </c>
       <c r="G125"/>
     </row>
-    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="86" t="s">
+    <row r="126" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A126" s="82" t="s">
         <v>571</v>
       </c>
       <c r="B126" s="36" t="s">
@@ -8944,8 +8944,8 @@
         <v>573</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A127" s="86" t="s">
+    <row r="127" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A127" s="82" t="s">
         <v>574</v>
       </c>
       <c r="B127" s="39" t="s">
@@ -8967,8 +8967,8 @@
         <v>576</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A128" s="86" t="s">
+    <row r="128" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A128" s="82" t="s">
         <v>577</v>
       </c>
       <c r="B128" s="36" t="s">
@@ -8990,8 +8990,8 @@
         <v>579</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A129" s="86" t="s">
+    <row r="129" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A129" s="82" t="s">
         <v>580</v>
       </c>
       <c r="B129" s="39" t="s">
@@ -9000,21 +9000,21 @@
       <c r="C129" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="D129" s="97" t="s">
+      <c r="D129" s="93" t="s">
         <v>582</v>
       </c>
-      <c r="E129" s="92" t="s">
+      <c r="E129" s="88" t="s">
+        <v>747</v>
+      </c>
+      <c r="F129" s="89" t="s">
+        <v>747</v>
+      </c>
+      <c r="G129" s="50" t="s">
         <v>748</v>
       </c>
-      <c r="F129" s="93" t="s">
-        <v>748</v>
-      </c>
-      <c r="G129" s="50" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A130" s="86" t="s">
+    </row>
+    <row r="130" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="82" t="s">
         <v>584</v>
       </c>
       <c r="B130" s="36" t="s">
@@ -9023,7 +9023,7 @@
       <c r="C130" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="D130" s="94" t="s">
+      <c r="D130" s="90" t="s">
         <v>584</v>
       </c>
       <c r="E130" s="38" t="s">
@@ -9036,8 +9036,8 @@
         <v>586</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="86" t="s">
+    <row r="131" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A131" s="82" t="s">
         <v>587</v>
       </c>
       <c r="B131" s="39" t="s">
@@ -9057,8 +9057,8 @@
         <v>589</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A132" s="86" t="s">
+    <row r="132" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="82" t="s">
         <v>590</v>
       </c>
       <c r="B132" s="36" t="s">
@@ -9070,18 +9070,18 @@
       <c r="D132" s="38" t="s">
         <v>590</v>
       </c>
-      <c r="E132" s="99" t="s">
+      <c r="E132" s="95" t="s">
         <v>592</v>
       </c>
-      <c r="F132" s="97" t="s">
+      <c r="F132" s="93" t="s">
         <v>592</v>
       </c>
       <c r="G132" s="48" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A133" s="86" t="s">
+    <row r="133" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A133" s="82" t="s">
         <v>594</v>
       </c>
       <c r="B133" s="39" t="s">
@@ -9101,8 +9101,8 @@
         <v>596</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="86" t="s">
+    <row r="134" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A134" s="82" t="s">
         <v>597</v>
       </c>
       <c r="B134" s="36" t="s">
@@ -9120,8 +9120,8 @@
       </c>
       <c r="G134"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="86" t="s">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" s="82" t="s">
         <v>599</v>
       </c>
       <c r="B135" s="39" t="s">
@@ -9137,8 +9137,8 @@
       </c>
       <c r="G135"/>
     </row>
-    <row r="136" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A136" s="86" t="s">
+    <row r="136" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A136" s="82" t="s">
         <v>601</v>
       </c>
       <c r="B136" s="36" t="s">
@@ -9156,8 +9156,8 @@
         <v>603</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="86" t="s">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="82" t="s">
         <v>604</v>
       </c>
       <c r="B137" s="39" t="s">
@@ -9173,8 +9173,8 @@
       </c>
       <c r="G137" s="53"/>
     </row>
-    <row r="138" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A138" s="86" t="s">
+    <row r="138" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A138" s="82" t="s">
         <v>606</v>
       </c>
       <c r="B138" s="36" t="s">
@@ -9192,8 +9192,8 @@
         <v>608</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A139" s="86" t="s">
+    <row r="139" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A139" s="82" t="s">
         <v>609</v>
       </c>
       <c r="B139" s="39" t="s">
@@ -9215,8 +9215,8 @@
         <v>611</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A140" s="86" t="s">
+    <row r="140" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A140" s="82" t="s">
         <v>612</v>
       </c>
       <c r="B140" s="36" t="s">
@@ -9233,15 +9233,15 @@
         <v>612</v>
       </c>
       <c r="G140" s="48" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" s="82" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="86" t="s">
+      <c r="B141" s="39" t="s">
         <v>615</v>
-      </c>
-      <c r="B141" s="39" t="s">
-        <v>616</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>233</v>
@@ -9249,349 +9249,349 @@
       <c r="D141" s="39"/>
       <c r="E141" s="39"/>
       <c r="F141" s="55" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G141" s="50" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A142" s="86" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142" s="82" t="s">
+        <v>616</v>
+      </c>
+      <c r="B142" s="36" t="s">
         <v>617</v>
-      </c>
-      <c r="B142" s="36" t="s">
-        <v>618</v>
       </c>
       <c r="C142" s="37" t="s">
         <v>233</v>
       </c>
       <c r="D142" s="36"/>
       <c r="E142" s="38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F142" s="52" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G142" s="48" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A143" s="82" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A143" s="86" t="s">
+      <c r="B143" s="39" t="s">
         <v>620</v>
       </c>
-      <c r="B143" s="39" t="s">
+      <c r="C143" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D143" s="39" t="s">
+        <v>619</v>
+      </c>
+      <c r="E143" s="41" t="s">
+        <v>619</v>
+      </c>
+      <c r="F143" s="89" t="s">
+        <v>619</v>
+      </c>
+      <c r="G143" s="50" t="s">
         <v>621</v>
       </c>
-      <c r="C143" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D143" s="39" t="s">
-        <v>620</v>
-      </c>
-      <c r="E143" s="41" t="s">
-        <v>620</v>
-      </c>
-      <c r="F143" s="93" t="s">
-        <v>620</v>
-      </c>
-      <c r="G143" s="50" t="s">
+    </row>
+    <row r="144" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A144" s="82" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A144" s="86" t="s">
+      <c r="B144" s="36" t="s">
         <v>623</v>
       </c>
-      <c r="B144" s="36" t="s">
+      <c r="C144" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D144" s="38" t="s">
+        <v>622</v>
+      </c>
+      <c r="E144" s="42" t="s">
+        <v>750</v>
+      </c>
+      <c r="F144" s="65" t="s">
+        <v>751</v>
+      </c>
+      <c r="G144" s="54" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A145" s="82" t="s">
         <v>624</v>
       </c>
-      <c r="C144" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D144" s="38" t="s">
-        <v>623</v>
-      </c>
-      <c r="E144" s="42" t="s">
-        <v>751</v>
-      </c>
-      <c r="F144" s="65" t="s">
-        <v>752</v>
-      </c>
-      <c r="G144" s="54" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A145" s="86" t="s">
+      <c r="B145" s="39" t="s">
         <v>625</v>
       </c>
-      <c r="B145" s="39" t="s">
+      <c r="C145" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D145" s="39"/>
+      <c r="E145" s="95" t="s">
         <v>626</v>
       </c>
-      <c r="C145" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D145" s="39"/>
-      <c r="E145" s="99" t="s">
+      <c r="F145" s="93" t="s">
+        <v>626</v>
+      </c>
+      <c r="G145" s="54" t="s">
         <v>627</v>
       </c>
-      <c r="F145" s="97" t="s">
-        <v>627</v>
-      </c>
-      <c r="G145" s="54" t="s">
+    </row>
+    <row r="146" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A146" s="82" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="86" t="s">
+      <c r="B146" s="36" t="s">
         <v>629</v>
-      </c>
-      <c r="B146" s="36" t="s">
-        <v>630</v>
       </c>
       <c r="C146" s="37" t="s">
         <v>252</v>
       </c>
       <c r="D146" s="36"/>
       <c r="E146" s="36" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F146" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G146" s="48" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A147" s="82" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A147" s="86" t="s">
+      <c r="B147" s="39" t="s">
         <v>632</v>
       </c>
-      <c r="B147" s="39" t="s">
+      <c r="C147" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D147" s="83" t="s">
+        <v>631</v>
+      </c>
+      <c r="E147" s="41" t="s">
+        <v>631</v>
+      </c>
+      <c r="F147" s="93" t="s">
         <v>633</v>
       </c>
-      <c r="C147" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D147" s="87" t="s">
-        <v>632</v>
-      </c>
-      <c r="E147" s="41" t="s">
-        <v>632</v>
-      </c>
-      <c r="F147" s="97" t="s">
+      <c r="G147" s="57" t="s">
         <v>634</v>
       </c>
-      <c r="G147" s="57" t="s">
+    </row>
+    <row r="148" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A148" s="82" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A148" s="86" t="s">
+      <c r="B148" s="36" t="s">
         <v>636</v>
       </c>
-      <c r="B148" s="36" t="s">
+      <c r="C148" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D148" s="36" t="s">
+        <v>635</v>
+      </c>
+      <c r="E148" s="38" t="s">
+        <v>635</v>
+      </c>
+      <c r="F148" s="52" t="s">
+        <v>635</v>
+      </c>
+      <c r="G148" s="48" t="s">
         <v>637</v>
       </c>
-      <c r="C148" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D148" s="36" t="s">
-        <v>636</v>
-      </c>
-      <c r="E148" s="38" t="s">
-        <v>636</v>
-      </c>
-      <c r="F148" s="52" t="s">
-        <v>636</v>
-      </c>
-      <c r="G148" s="48" t="s">
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A149" s="82" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="86" t="s">
+      <c r="B149" s="39" t="s">
         <v>639</v>
       </c>
-      <c r="B149" s="39" t="s">
+      <c r="C149" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D149" s="39" t="s">
+        <v>638</v>
+      </c>
+      <c r="E149" s="39" t="s">
+        <v>638</v>
+      </c>
+      <c r="F149" s="51" t="s">
+        <v>638</v>
+      </c>
+      <c r="G149" s="50" t="s">
         <v>640</v>
       </c>
-      <c r="C149" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D149" s="39" t="s">
-        <v>639</v>
-      </c>
-      <c r="E149" s="39" t="s">
-        <v>639</v>
-      </c>
-      <c r="F149" s="51" t="s">
-        <v>639</v>
-      </c>
-      <c r="G149" s="50" t="s">
+    </row>
+    <row r="150" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A150" s="82" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A150" s="86" t="s">
+      <c r="B150" s="36" t="s">
         <v>642</v>
-      </c>
-      <c r="B150" s="36" t="s">
-        <v>643</v>
       </c>
       <c r="C150" s="37" t="s">
         <v>233</v>
       </c>
       <c r="D150" s="36"/>
       <c r="E150" s="42" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F150" s="52" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G150" s="48" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A151" s="82" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="86" t="s">
+      <c r="B151" s="39" t="s">
         <v>645</v>
-      </c>
-      <c r="B151" s="39" t="s">
-        <v>646</v>
       </c>
       <c r="C151" s="40" t="s">
         <v>252</v>
       </c>
       <c r="D151" s="39"/>
       <c r="E151" s="41" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F151" s="51" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G151" s="50" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152" s="82" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="86" t="s">
+      <c r="B152" s="36" t="s">
         <v>648</v>
-      </c>
-      <c r="B152" s="36" t="s">
-        <v>649</v>
       </c>
       <c r="C152" s="37" t="s">
         <v>233</v>
       </c>
       <c r="D152" s="36"/>
       <c r="E152" s="36" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F152" s="52" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G152" s="48" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="86" t="s">
+    <row r="153" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A153" s="82" t="s">
+        <v>649</v>
+      </c>
+      <c r="B153" s="39" t="s">
         <v>650</v>
       </c>
-      <c r="B153" s="39" t="s">
+      <c r="C153" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D153" s="39" t="s">
+        <v>649</v>
+      </c>
+      <c r="E153" s="39" t="s">
+        <v>649</v>
+      </c>
+      <c r="F153" s="51" t="s">
+        <v>649</v>
+      </c>
+      <c r="G153" s="48" t="s">
         <v>651</v>
       </c>
-      <c r="C153" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D153" s="39" t="s">
-        <v>650</v>
-      </c>
-      <c r="E153" s="39" t="s">
-        <v>650</v>
-      </c>
-      <c r="F153" s="51" t="s">
-        <v>650</v>
-      </c>
-      <c r="G153" s="48" t="s">
+    </row>
+    <row r="154" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A154" s="82" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A154" s="86" t="s">
+      <c r="B154" s="36" t="s">
         <v>653</v>
       </c>
-      <c r="B154" s="36" t="s">
-        <v>654</v>
-      </c>
       <c r="C154" s="37" t="s">
         <v>233</v>
       </c>
       <c r="D154" s="36" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E154" s="36" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F154" s="52" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G154" s="48" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A155" s="86" t="s">
+    <row r="155" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A155" s="82" t="s">
+        <v>654</v>
+      </c>
+      <c r="B155" s="39" t="s">
         <v>655</v>
       </c>
-      <c r="B155" s="39" t="s">
-        <v>656</v>
-      </c>
       <c r="C155" s="40" t="s">
         <v>233</v>
       </c>
       <c r="D155" s="39" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E155" s="39" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F155" s="51" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G155" s="48" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" s="86" t="s">
+    <row r="156" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A156" s="82" t="s">
+        <v>656</v>
+      </c>
+      <c r="B156" s="36" t="s">
         <v>657</v>
-      </c>
-      <c r="B156" s="36" t="s">
-        <v>658</v>
       </c>
       <c r="C156" s="37" t="s">
         <v>233</v>
       </c>
       <c r="D156" s="36"/>
       <c r="E156" s="38" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F156" s="65" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G156" s="48" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A157" s="82" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A157" s="86" t="s">
+      <c r="B157" s="39" t="s">
         <v>660</v>
-      </c>
-      <c r="B157" s="39" t="s">
-        <v>661</v>
       </c>
       <c r="C157" s="40" t="s">
         <v>233</v>
@@ -9599,177 +9599,177 @@
       <c r="D157" s="39"/>
       <c r="E157" s="39"/>
       <c r="F157" s="51" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G157" s="48" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A158" s="82" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A158" s="86" t="s">
+      <c r="B158" s="36" t="s">
         <v>663</v>
-      </c>
-      <c r="B158" s="36" t="s">
-        <v>664</v>
       </c>
       <c r="C158" s="37" t="s">
         <v>233</v>
       </c>
       <c r="D158" s="36"/>
       <c r="E158" s="38" t="s">
-        <v>663</v>
-      </c>
-      <c r="F158" s="101" t="s">
-        <v>663</v>
+        <v>662</v>
+      </c>
+      <c r="F158" s="97" t="s">
+        <v>662</v>
       </c>
       <c r="G158" s="48" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A159" s="82" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="86" t="s">
+      <c r="B159" s="39" t="s">
         <v>666</v>
       </c>
-      <c r="B159" s="39" t="s">
-        <v>667</v>
-      </c>
       <c r="C159" s="40" t="s">
         <v>233</v>
       </c>
       <c r="D159" s="39" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E159" s="39" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F159" s="51" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G159" s="48" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A160" s="86" t="s">
+    <row r="160" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A160" s="82" t="s">
+        <v>667</v>
+      </c>
+      <c r="B160" s="36" t="s">
         <v>668</v>
       </c>
-      <c r="B160" s="36" t="s">
+      <c r="C160" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D160" s="36" t="s">
+        <v>667</v>
+      </c>
+      <c r="E160" s="36" t="s">
+        <v>667</v>
+      </c>
+      <c r="F160" s="49" t="s">
+        <v>667</v>
+      </c>
+      <c r="G160" s="58" t="s">
         <v>669</v>
       </c>
-      <c r="C160" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D160" s="36" t="s">
-        <v>668</v>
-      </c>
-      <c r="E160" s="36" t="s">
-        <v>668</v>
-      </c>
-      <c r="F160" s="49" t="s">
-        <v>668</v>
-      </c>
-      <c r="G160" s="58" t="s">
+    </row>
+    <row r="161" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A161" s="82" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A161" s="86" t="s">
+      <c r="B161" s="39" t="s">
         <v>671</v>
       </c>
-      <c r="B161" s="39" t="s">
+      <c r="C161" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D161" s="39" t="s">
+        <v>670</v>
+      </c>
+      <c r="E161" s="93" t="s">
         <v>672</v>
       </c>
-      <c r="C161" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D161" s="39" t="s">
-        <v>671</v>
-      </c>
-      <c r="E161" s="97" t="s">
+      <c r="F161" s="84" t="s">
+        <v>753</v>
+      </c>
+      <c r="G161" s="48" t="s">
         <v>673</v>
       </c>
-      <c r="F161" s="88" t="s">
+    </row>
+    <row r="162" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A162" s="82" t="s">
+        <v>674</v>
+      </c>
+      <c r="B162" s="36" t="s">
+        <v>675</v>
+      </c>
+      <c r="C162" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D162" s="38" t="s">
+        <v>674</v>
+      </c>
+      <c r="E162" s="90" t="s">
         <v>754</v>
       </c>
-      <c r="G161" s="48" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="86" t="s">
-        <v>675</v>
-      </c>
-      <c r="B162" s="36" t="s">
+      <c r="F162" s="97" t="s">
+        <v>754</v>
+      </c>
+      <c r="G162" s="48" t="s">
         <v>676</v>
       </c>
-      <c r="C162" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D162" s="38" t="s">
-        <v>675</v>
-      </c>
-      <c r="E162" s="94" t="s">
+    </row>
+    <row r="163" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A163" s="82" t="s">
+        <v>677</v>
+      </c>
+      <c r="B163" s="39" t="s">
+        <v>678</v>
+      </c>
+      <c r="C163" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D163" s="39" t="s">
+        <v>677</v>
+      </c>
+      <c r="E163" s="83" t="s">
         <v>755</v>
       </c>
-      <c r="F162" s="101" t="s">
+      <c r="F163" s="84" t="s">
         <v>755</v>
       </c>
-      <c r="G162" s="48" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A163" s="86" t="s">
-        <v>678</v>
-      </c>
-      <c r="B163" s="39" t="s">
+      <c r="G163" s="48" t="s">
         <v>679</v>
       </c>
-      <c r="C163" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D163" s="39" t="s">
-        <v>678</v>
-      </c>
-      <c r="E163" s="87" t="s">
-        <v>756</v>
-      </c>
-      <c r="F163" s="88" t="s">
-        <v>756</v>
-      </c>
-      <c r="G163" s="48" t="s">
+    </row>
+    <row r="164" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A164" s="82" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A164" s="86" t="s">
+      <c r="B164" s="36" t="s">
         <v>681</v>
       </c>
-      <c r="B164" s="36" t="s">
+      <c r="C164" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D164" s="36" t="s">
+        <v>680</v>
+      </c>
+      <c r="E164" s="36" t="s">
+        <v>680</v>
+      </c>
+      <c r="F164" s="93" t="s">
         <v>682</v>
       </c>
-      <c r="C164" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D164" s="36" t="s">
-        <v>681</v>
-      </c>
-      <c r="E164" s="36" t="s">
-        <v>681</v>
-      </c>
-      <c r="F164" s="97" t="s">
+      <c r="G164" s="48" t="s">
         <v>683</v>
       </c>
-      <c r="G164" s="48" t="s">
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A165" s="82" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="86" t="s">
+      <c r="B165" s="39" t="s">
         <v>685</v>
-      </c>
-      <c r="B165" s="39" t="s">
-        <v>686</v>
       </c>
       <c r="C165" s="40" t="s">
         <v>233</v>
@@ -9777,138 +9777,138 @@
       <c r="D165" s="39"/>
       <c r="E165" s="39"/>
       <c r="F165" s="51" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G165" s="48" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A166" s="86" t="s">
+    <row r="166" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A166" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="B166" s="36" t="s">
         <v>687</v>
       </c>
-      <c r="B166" s="36" t="s">
+      <c r="C166" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D166" s="36"/>
+      <c r="E166" s="90" t="s">
+        <v>756</v>
+      </c>
+      <c r="F166" s="97" t="s">
+        <v>757</v>
+      </c>
+      <c r="G166" s="48" t="s">
         <v>688</v>
       </c>
-      <c r="C166" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D166" s="36"/>
-      <c r="E166" s="94" t="s">
-        <v>757</v>
-      </c>
-      <c r="F166" s="101" t="s">
-        <v>758</v>
-      </c>
-      <c r="G166" s="48" t="s">
+    </row>
+    <row r="167" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A167" s="82" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="86" t="s">
+      <c r="B167" s="39" t="s">
         <v>690</v>
-      </c>
-      <c r="B167" s="39" t="s">
-        <v>691</v>
       </c>
       <c r="C167" s="40" t="s">
         <v>252</v>
       </c>
       <c r="D167" s="39"/>
-      <c r="E167" s="87" t="s">
-        <v>759</v>
-      </c>
-      <c r="F167" s="88" t="s">
-        <v>759</v>
+      <c r="E167" s="83" t="s">
+        <v>758</v>
+      </c>
+      <c r="F167" s="84" t="s">
+        <v>758</v>
       </c>
       <c r="G167" s="48" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="86" t="s">
+    <row r="168" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A168" s="82" t="s">
+        <v>691</v>
+      </c>
+      <c r="B168" s="36" t="s">
         <v>692</v>
-      </c>
-      <c r="B168" s="36" t="s">
-        <v>693</v>
       </c>
       <c r="C168" s="37" t="s">
         <v>233</v>
       </c>
       <c r="D168" s="36"/>
       <c r="E168" s="38" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F168" s="52" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G168" s="48" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A169" s="82" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="86" t="s">
+      <c r="B169" s="39" t="s">
         <v>695</v>
-      </c>
-      <c r="B169" s="39" t="s">
-        <v>696</v>
       </c>
       <c r="C169" s="40" t="s">
         <v>252</v>
       </c>
       <c r="D169" s="39"/>
       <c r="E169" s="41" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F169" s="51" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G169" s="48" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A170" s="82" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="86" t="s">
+      <c r="B170" s="36" t="s">
         <v>698</v>
-      </c>
-      <c r="B170" s="36" t="s">
-        <v>699</v>
       </c>
       <c r="C170" s="37" t="s">
         <v>252</v>
       </c>
       <c r="D170" s="36" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E170" s="36" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F170" s="52" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G170" s="48" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" s="86" t="s">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A171" s="82" t="s">
+        <v>699</v>
+      </c>
+      <c r="B171" s="44" t="s">
         <v>700</v>
-      </c>
-      <c r="B171" s="44" t="s">
-        <v>701</v>
       </c>
       <c r="C171" s="45" t="s">
         <v>233</v>
       </c>
       <c r="D171" s="44"/>
       <c r="E171" s="46" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F171" s="56" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G171" s="48" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
   </sheetData>
@@ -9917,12 +9917,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001FF3CDC142E59F46976220B5CA0CB5FC" ma:contentTypeVersion="2" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="0b8a8c1c321c01bcbeb872dfd6c1bb21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78bd1115-c349-4e94-811d-d06a7ae9090b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4ae236ed4d02964ec2f225fff35efa2" ns2:_="">
     <xsd:import namespace="78bd1115-c349-4e94-811d-d06a7ae9090b"/>
@@ -10054,6 +10048,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10064,16 +10064,30 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FC4447-7B71-48E8-91FE-1A5150E609C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="78bd1115-c349-4e94-811d-d06a7ae9090b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1D9392E-2A4B-45BA-8B16-B0D40262D09F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FC4447-7B71-48E8-91FE-1A5150E609C7}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>